<commit_message>
borrado de clientes al importar funcionando
</commit_message>
<xml_diff>
--- a/clientes_exportados.xlsx
+++ b/clientes_exportados.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes_exportados" sheetId="1" r:id="rId1"/>
+    <sheet name="clientes_exportados" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -48,15 +44,15 @@
     <t>ANTONIO MARIÑO CARRION</t>
   </si>
   <si>
-    <t>TERESA BERTRAN PAREJO</t>
-  </si>
-  <si>
     <t>ALBA MUÑOZ MONTSERRAT</t>
   </si>
   <si>
     <t>DANIEL BERNAT SOBRINO</t>
   </si>
   <si>
+    <t>añadido importado</t>
+  </si>
+  <si>
     <t>María Navarro Velazquez</t>
   </si>
   <si>
@@ -103,9 +99,6 @@
   </si>
   <si>
     <t>qwerty</t>
-  </si>
-  <si>
-    <t>prueba contacto refresg</t>
   </si>
   <si>
     <t>remodificado</t>
@@ -132,9 +125,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -145,29 +143,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -457,14 +454,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -526,13 +526,13 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3">
-        <v>876543987</v>
+        <v>564387267</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -549,13 +549,13 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>564387267</v>
+        <v>904858234</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -572,13 +572,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5">
-        <v>904858234</v>
+        <v>3333333</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -595,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -652,48 +652,48 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>987654321</v>
+        <v>984502393</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C10">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G10">
-        <v>12313</v>
+        <v>984502393</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -710,13 +710,13 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G11">
-        <v>555555555</v>
+        <v>987654321</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -733,13 +733,13 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G12">
-        <v>12123</v>
+        <v>12313</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -756,295 +756,577 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G13">
-        <v>123123</v>
+        <v>555555555</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>19</v>
-      </c>
-      <c r="F14">
-        <v>123</v>
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>123</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G15">
-        <v>1231321321</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G16">
-        <v>13123123</v>
+        <v>12313</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G17">
-        <v>123</v>
+        <v>555555555</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G18">
-        <v>242432</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G19">
-        <v>12341234</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C20">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G20">
-        <v>123123123</v>
+        <v>12313</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <v>456</v>
+        <v>654321987</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>36</v>
-      </c>
-      <c r="F21">
-        <v>123</v>
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
       </c>
       <c r="G21">
-        <v>2123</v>
+        <v>555555555</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C22">
-        <v>456</v>
+        <v>654321987</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>37</v>
-      </c>
-      <c r="F22">
-        <v>123132</v>
+        <v>66</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
       </c>
       <c r="G22">
-        <v>123123</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C23">
-        <v>555777999</v>
+        <v>654321987</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23">
+        <v>123123</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>645678954</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24">
+        <v>123</v>
+      </c>
+      <c r="G24">
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>20189596</v>
+        <v>645678954</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <v>1231321321</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>87767766</v>
+        <v>645678954</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26">
+        <v>13123123</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>242432</v>
+        <v>645678954</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27">
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>645678954</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28">
+        <v>242432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>645678954</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29">
+        <v>12341234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>456</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>36</v>
+      </c>
+      <c r="F30">
+        <v>123</v>
+      </c>
+      <c r="G30">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>456</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>37</v>
+      </c>
+      <c r="F31">
+        <v>123132</v>
+      </c>
+      <c r="G31">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>456</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>59</v>
+      </c>
+      <c r="F32">
+        <v>123132</v>
+      </c>
+      <c r="G32">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33">
+        <v>456</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>74</v>
+      </c>
+      <c r="F33">
+        <v>123132</v>
+      </c>
+      <c r="G33">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>555777999</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
         <v>31</v>
       </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28">
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>20189596</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37">
+        <v>87767766</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>242432</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
         <v>33333</v>
       </c>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
borrado clientes y contactos al importar funcionando
</commit_message>
<xml_diff>
--- a/clientes_exportados.xlsx
+++ b/clientes_exportados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -44,15 +44,15 @@
     <t>ANTONIO MARIÑO CARRION</t>
   </si>
   <si>
+    <t>TERESA BERTRAN PAREJO</t>
+  </si>
+  <si>
     <t>ALBA MUÑOZ MONTSERRAT</t>
   </si>
   <si>
     <t>DANIEL BERNAT SOBRINO</t>
   </si>
   <si>
-    <t>añadido importado</t>
-  </si>
-  <si>
     <t>María Navarro Velazquez</t>
   </si>
   <si>
@@ -101,6 +101,9 @@
     <t>qwerty</t>
   </si>
   <si>
+    <t>prueba contacto refresg</t>
+  </si>
+  <si>
     <t>remodificado</t>
   </si>
   <si>
@@ -119,7 +122,16 @@
     <t>Alta 6 de Abril de 2018</t>
   </si>
   <si>
-    <t>modificación importando</t>
+    <t>Hola que tal</t>
+  </si>
+  <si>
+    <t>qweqwe</t>
+  </si>
+  <si>
+    <t>Victor 2123</t>
+  </si>
+  <si>
+    <t>borrado</t>
   </si>
 </sst>
 </file>
@@ -458,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,13 +538,13 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3">
-        <v>564387267</v>
+        <v>876543987</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -549,13 +561,13 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>904858234</v>
+        <v>564387267</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -572,13 +584,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5">
-        <v>3333333</v>
+        <v>904858234</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -595,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
@@ -652,48 +664,48 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>654321987</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>645678954</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>48</v>
-      </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G9">
-        <v>984502393</v>
+        <v>987654321</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>645678954</v>
+        <v>654321987</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G10">
-        <v>984502393</v>
+        <v>12313</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -710,13 +722,13 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G11">
-        <v>987654321</v>
+        <v>555555555</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -733,13 +745,13 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>12313</v>
+        <v>12123</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -756,564 +768,349 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13">
-        <v>555555555</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>123</v>
       </c>
       <c r="G14">
-        <v>12123</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G15">
-        <v>123123</v>
+        <v>1231321321</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G16">
-        <v>12313</v>
+        <v>13123123</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G17">
-        <v>555555555</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G18">
-        <v>12123</v>
+        <v>242432</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G19">
-        <v>123123</v>
+        <v>12341234</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>654321987</v>
+        <v>645678954</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>12313</v>
+        <v>123123123</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C21">
-        <v>654321987</v>
+        <v>456</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>65</v>
-      </c>
-      <c r="F21" t="s">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="F21">
+        <v>123</v>
       </c>
       <c r="G21">
-        <v>555555555</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>654321987</v>
+        <v>456</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="F22">
+        <v>123132</v>
       </c>
       <c r="G22">
-        <v>12123</v>
+        <v>123123</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>654321987</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>67</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23">
-        <v>123123</v>
-      </c>
+        <v>555777999</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>645678954</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>19</v>
-      </c>
-      <c r="F24">
-        <v>123</v>
-      </c>
-      <c r="G24">
-        <v>123</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C25">
-        <v>645678954</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25">
-        <v>1231321321</v>
-      </c>
+        <v>20189596</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C26">
-        <v>645678954</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>21</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26">
-        <v>13123123</v>
-      </c>
+        <v>87767766</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C27">
-        <v>645678954</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>22</v>
-      </c>
-      <c r="F27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27">
         <v>123</v>
       </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>645678954</v>
-      </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28">
-        <v>25</v>
-      </c>
-      <c r="F28" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28">
         <v>242432</v>
       </c>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C29">
-        <v>645678954</v>
-      </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-      <c r="E29">
-        <v>27</v>
-      </c>
-      <c r="F29" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29">
-        <v>12341234</v>
-      </c>
+        <v>132123</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C30">
-        <v>456</v>
+        <v>123123</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E30">
-        <v>36</v>
-      </c>
-      <c r="F30">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30">
         <v>123</v>
       </c>
-      <c r="G30">
-        <v>2123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31">
-        <v>456</v>
-      </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <v>37</v>
-      </c>
-      <c r="F31">
-        <v>123132</v>
-      </c>
-      <c r="G31">
-        <v>123123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32">
-        <v>456</v>
-      </c>
-      <c r="D32">
-        <v>5</v>
-      </c>
-      <c r="E32">
-        <v>59</v>
-      </c>
-      <c r="F32">
-        <v>123132</v>
-      </c>
-      <c r="G32">
-        <v>123123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33">
-        <v>456</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33">
-        <v>74</v>
-      </c>
-      <c r="F33">
-        <v>123132</v>
-      </c>
-      <c r="G33">
-        <v>123123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34">
-        <v>9</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34">
-        <v>555777999</v>
-      </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36">
-        <v>20189596</v>
-      </c>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37">
-        <v>87767766</v>
-      </c>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38">
-        <v>27</v>
-      </c>
-      <c r="B38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38">
-        <v>242432</v>
-      </c>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39">
-        <v>33333</v>
-      </c>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
importacion insert update clientes funcionando
solo falta insert y update de contactos
</commit_message>
<xml_diff>
--- a/clientes_exportados.xlsx
+++ b/clientes_exportados.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes_exportados" sheetId="1" r:id="rId4"/>
+    <sheet name="clientes_exportados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -122,9 +126,6 @@
     <t>Alta 6 de Abril de 2018</t>
   </si>
   <si>
-    <t>Hola que tal</t>
-  </si>
-  <si>
     <t>qweqwe</t>
   </si>
   <si>
@@ -132,19 +133,17 @@
   </si>
   <si>
     <t>borrado</t>
+  </si>
+  <si>
+    <t>Hi how are you</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -155,28 +154,29 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -466,17 +466,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -994,10 +991,6 @@
       <c r="C23">
         <v>555777999</v>
       </c>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
@@ -1009,10 +1002,6 @@
       <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
@@ -1024,10 +1013,6 @@
       <c r="C25">
         <v>20189596</v>
       </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
@@ -1039,91 +1024,70 @@
       <c r="C26">
         <v>87767766</v>
       </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
       <c r="C27">
-        <v>123</v>
-      </c>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
+        <v>242432</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>242432</v>
-      </c>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
+        <v>132123</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="C29">
-        <v>132123</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
+        <v>123123</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30">
-        <v>123123</v>
-      </c>
-      <c r="D30">
-        <v>29</v>
-      </c>
-      <c r="E30">
-        <v>43</v>
-      </c>
-      <c r="F30" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30">
-        <v>123</v>
+        <v>55555</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Errores JQuery e importación solucionados
</commit_message>
<xml_diff>
--- a/clientes_exportados.xlsx
+++ b/clientes_exportados.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes_exportados" sheetId="1" r:id="rId1"/>
+    <sheet name="clientes_exportados" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -130,20 +126,19 @@
   </si>
   <si>
     <t>Victor 2123</t>
-  </si>
-  <si>
-    <t>borrado</t>
-  </si>
-  <si>
-    <t>importado excel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -154,29 +149,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -466,14 +460,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -991,6 +988,10 @@
       <c r="C23">
         <v>555777999</v>
       </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
@@ -1002,6 +1003,10 @@
       <c r="C24" t="s">
         <v>32</v>
       </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
@@ -1013,6 +1018,10 @@
       <c r="C25">
         <v>20189596</v>
       </c>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
@@ -1024,6 +1033,10 @@
       <c r="C26">
         <v>87767766</v>
       </c>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
@@ -1035,10 +1048,14 @@
       <c r="C27">
         <v>242432</v>
       </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
@@ -1046,22 +1063,14 @@
       <c r="C28">
         <v>132123</v>
       </c>
-      <c r="D28">
-        <v>28</v>
-      </c>
-      <c r="E28">
-        <v>44</v>
-      </c>
-      <c r="F28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28">
-        <v>22222</v>
-      </c>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
@@ -1069,26 +1078,23 @@
       <c r="C29">
         <v>123123</v>
       </c>
-      <c r="D29">
-        <v>29</v>
-      </c>
-      <c r="E29">
-        <v>43</v>
-      </c>
-      <c r="F29" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29">
-        <v>123</v>
-      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>